<commit_message>
Support File Extension in Excel
</commit_message>
<xml_diff>
--- a/xreplace.xlsx
+++ b/xreplace.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Xreplace" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Yreplace" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="File" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Find</t>
   </si>
@@ -60,6 +61,33 @@
   </si>
   <si>
     <t xml:space="preserve">Findsdfxxsscd 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.css</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.liquid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.phtml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.less</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.xml</t>
   </si>
 </sst>
 </file>
@@ -69,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -90,11 +118,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,7 +162,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,18 +179,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,7 +199,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,10 +229,10 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -270,15 +281,15 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:A"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -288,7 +299,7 @@
       <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -299,12 +310,9 @@
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
@@ -325,7 +333,7 @@
       <c r="A9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -340,6 +348,78 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.38"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>